<commit_message>
Got Excel input started and made print control.
</commit_message>
<xml_diff>
--- a/SleepDiaryTemplate.xlsx
+++ b/SleepDiaryTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mwhites/PycharmProjects/SleepDB2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew\Documents\Programming\Python\SleepDB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2299BD71-4E59-3447-BF89-E5DFF1346D77}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE82A290-F9C2-4D53-88D3-1620BCE38C29}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="220" yWindow="1120" windowWidth="21940" windowHeight="16320" xr2:uid="{8E52F8CF-E89F-C141-ABDD-CEBCAC2EF7FA}"/>
+    <workbookView xWindow="8835" yWindow="930" windowWidth="15315" windowHeight="13140" xr2:uid="{8E52F8CF-E89F-C141-ABDD-CEBCAC2EF7FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -120,7 +120,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -129,6 +129,11 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -443,94 +448,137 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE1D3074-87B5-B943-B3EA-8EB0EDF50BC8}">
-  <dimension ref="A1:XFD15"/>
+  <dimension ref="A1:XFC15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37.5" customWidth="1"/>
-    <col min="2" max="9" width="33.1640625" customWidth="1"/>
-    <col min="10" max="16383" width="10.83203125" hidden="1"/>
-    <col min="16384" max="16384" width="43.83203125" hidden="1" customWidth="1"/>
+    <col min="2" max="9" width="33.125" customWidth="1"/>
+    <col min="10" max="16383" width="10.875" hidden="1"/>
+    <col min="16384" max="16384" width="43.875" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" ht="53" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+    </row>
+    <row r="2" spans="1:6" ht="53.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+    </row>
+    <row r="8" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B8" s="8"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" ht="120" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+    </row>
+    <row r="12" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B14" s="6"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
+      <c r="B15" s="6"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>